<commit_message>
Updating attendance files 24th feb
</commit_message>
<xml_diff>
--- a/attendance-files/FIM/FIM-U (ABCD) Attendance Sheet.xlsx
+++ b/attendance-files/FIM/FIM-U (ABCD) Attendance Sheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="162">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -942,6 +942,9 @@
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -956,9 +959,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="F7" s="25">
         <f t="shared" ref="F7:F95" si="2">IF(D7&gt;0,COUNTIF(G7:Z7,"P"),"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>20</v>
@@ -1630,27 +1630,31 @@
       <c r="P7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
-      <c r="AA7" s="28"/>
+      <c r="Q7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="29">
+      <c r="A8" s="30">
         <f t="shared" ref="A8:A95" si="3">IF(B8&gt;0,A7+1,"")</f>
         <v>2</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1660,20 +1664,20 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F8" s="32">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="34" t="s">
+      <c r="F8" s="33">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="26" t="s">
@@ -1688,14 +1692,18 @@
       <c r="N8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
+      <c r="O8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
       <c r="U8" s="35"/>
@@ -1707,14 +1715,14 @@
       <c r="AA8" s="35"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="29">
+      <c r="A9" s="30">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="13" t="s">
@@ -1722,11 +1730,11 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G9" s="26" t="s">
         <v>20</v>
@@ -1758,8 +1766,12 @@
       <c r="P9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
+      <c r="Q9" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
       <c r="U9" s="35"/>
@@ -1771,14 +1783,14 @@
       <c r="AA9" s="35"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="29">
+      <c r="A10" s="30">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -1786,11 +1798,11 @@
       </c>
       <c r="E10" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F10" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F10" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>20</v>
@@ -1810,10 +1822,10 @@
       <c r="L10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="34" t="s">
+      <c r="M10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O10" s="27" t="s">
@@ -1822,8 +1834,12 @@
       <c r="P10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
+      <c r="Q10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
       <c r="U10" s="35"/>
@@ -1835,14 +1851,14 @@
       <c r="AA10" s="35"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="29">
+      <c r="A11" s="30">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="32" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -1852,14 +1868,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F11" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F11" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="26" t="s">
@@ -1886,8 +1902,12 @@
       <c r="P11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
+      <c r="Q11" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
       <c r="U11" s="35"/>
@@ -1899,14 +1919,14 @@
       <c r="AA11" s="35"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="29">
+      <c r="A12" s="30">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -1914,11 +1934,11 @@
       </c>
       <c r="E12" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F12" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F12" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G12" s="26" t="s">
         <v>20</v>
@@ -1929,7 +1949,7 @@
       <c r="I12" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="26" t="s">
@@ -1947,11 +1967,15 @@
       <c r="O12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
+      <c r="P12" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
       <c r="U12" s="35"/>
@@ -1963,14 +1987,14 @@
       <c r="AA12" s="35"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="29">
+      <c r="A13" s="30">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -1980,14 +2004,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F13" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F13" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="26" t="s">
@@ -2011,11 +2035,15 @@
       <c r="O13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
+      <c r="P13" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
@@ -2027,14 +2055,14 @@
       <c r="AA13" s="35"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="29">
+      <c r="A14" s="30">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="32" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="13" t="s">
@@ -2044,9 +2072,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F14" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="F14" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G14" s="26" t="s">
         <v>20</v>
@@ -2057,7 +2085,7 @@
       <c r="I14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="26" t="s">
@@ -2066,10 +2094,10 @@
       <c r="L14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="34" t="s">
+      <c r="M14" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O14" s="27" t="s">
@@ -2078,8 +2106,12 @@
       <c r="P14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
+      <c r="Q14" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S14" s="35"/>
       <c r="T14" s="35"/>
       <c r="U14" s="35"/>
@@ -2091,14 +2123,14 @@
       <c r="AA14" s="35"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="29">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="30">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2108,9 +2140,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F15" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F15" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G15" s="26" t="s">
         <v>20</v>
@@ -2124,7 +2156,7 @@
       <c r="J15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="34" t="s">
+      <c r="K15" s="28" t="s">
         <v>23</v>
       </c>
       <c r="L15" s="26" t="s">
@@ -2139,11 +2171,15 @@
       <c r="O15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
+      <c r="P15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q15" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S15" s="35"/>
       <c r="T15" s="35"/>
       <c r="U15" s="35"/>
@@ -2155,14 +2191,14 @@
       <c r="AA15" s="35"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="29">
+      <c r="A16" s="30">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="32" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -2172,9 +2208,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F16" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="F16" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G16" s="26" t="s">
         <v>20</v>
@@ -2182,7 +2218,7 @@
       <c r="H16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J16" s="26" t="s">
@@ -2200,14 +2236,18 @@
       <c r="N16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P16" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
+      <c r="O16" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R16" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S16" s="35"/>
       <c r="T16" s="35"/>
       <c r="U16" s="35"/>
@@ -2219,14 +2259,14 @@
       <c r="AA16" s="35"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="29">
+      <c r="A17" s="30">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -2236,9 +2276,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F17" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F17" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G17" s="26" t="s">
         <v>20</v>
@@ -2261,7 +2301,7 @@
       <c r="M17" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O17" s="27" t="s">
@@ -2270,8 +2310,12 @@
       <c r="P17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
+      <c r="Q17" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S17" s="35"/>
       <c r="T17" s="35"/>
       <c r="U17" s="35"/>
@@ -2283,14 +2327,14 @@
       <c r="AA17" s="35"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="29">
+      <c r="A18" s="30">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -2300,9 +2344,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F18" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="F18" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G18" s="26" t="s">
         <v>20</v>
@@ -2319,23 +2363,27 @@
       <c r="K18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L18" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P18" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
+      <c r="P18" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
       <c r="U18" s="35"/>
@@ -2347,14 +2395,14 @@
       <c r="AA18" s="35"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="29">
+      <c r="A19" s="30">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="32" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2364,9 +2412,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F19" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G19" s="26" t="s">
         <v>20</v>
@@ -2398,8 +2446,12 @@
       <c r="P19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
+      <c r="Q19" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R19" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
       <c r="U19" s="35"/>
@@ -2411,14 +2463,14 @@
       <c r="AA19" s="35"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="29">
+      <c r="A20" s="30">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="32" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -2428,9 +2480,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F20" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F20" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G20" s="26" t="s">
         <v>20</v>
@@ -2462,8 +2514,12 @@
       <c r="P20" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
+      <c r="Q20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S20" s="35"/>
       <c r="T20" s="35"/>
       <c r="U20" s="35"/>
@@ -2475,14 +2531,14 @@
       <c r="AA20" s="35"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="29">
+      <c r="A21" s="30">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="13" t="s">
@@ -2492,9 +2548,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F21" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F21" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G21" s="26" t="s">
         <v>20</v>
@@ -2514,10 +2570,10 @@
       <c r="L21" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M21" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N21" s="34" t="s">
+      <c r="M21" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O21" s="27" t="s">
@@ -2526,8 +2582,12 @@
       <c r="P21" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
+      <c r="Q21" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R21" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S21" s="35"/>
       <c r="T21" s="35"/>
       <c r="U21" s="35"/>
@@ -2539,14 +2599,14 @@
       <c r="AA21" s="35"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="29">
+      <c r="A22" s="30">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2556,9 +2616,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F22" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F22" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G22" s="26" t="s">
         <v>20</v>
@@ -2569,7 +2629,7 @@
       <c r="I22" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="26" t="s">
@@ -2590,8 +2650,12 @@
       <c r="P22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
+      <c r="Q22" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S22" s="35"/>
       <c r="T22" s="35"/>
       <c r="U22" s="35"/>
@@ -2603,14 +2667,14 @@
       <c r="AA22" s="35"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="29">
+      <c r="A23" s="30">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="32" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="13" t="s">
@@ -2620,9 +2684,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F23" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F23" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G23" s="26" t="s">
         <v>20</v>
@@ -2639,7 +2703,7 @@
       <c r="K23" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="34" t="s">
+      <c r="L23" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M23" s="26" t="s">
@@ -2654,8 +2718,12 @@
       <c r="P23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
+      <c r="Q23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S23" s="35"/>
       <c r="T23" s="35"/>
       <c r="U23" s="35"/>
@@ -2667,14 +2735,14 @@
       <c r="AA23" s="35"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="29">
+      <c r="A24" s="30">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="32" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="13" t="s">
@@ -2682,9 +2750,9 @@
       </c>
       <c r="E24" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="32">
+        <v>3</v>
+      </c>
+      <c r="F24" s="33">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -2706,7 +2774,7 @@
       <c r="L24" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N24" s="27" t="s">
@@ -2718,8 +2786,12 @@
       <c r="P24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
+      <c r="Q24" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S24" s="35"/>
       <c r="T24" s="35"/>
       <c r="U24" s="35"/>
@@ -2731,14 +2803,14 @@
       <c r="AA24" s="35"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="29">
+      <c r="A25" s="30">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="32" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="13" t="s">
@@ -2746,16 +2818,16 @@
       </c>
       <c r="E25" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F25" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F25" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="26" t="s">
@@ -2782,8 +2854,12 @@
       <c r="P25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
+      <c r="Q25" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S25" s="35"/>
       <c r="T25" s="35"/>
       <c r="U25" s="35"/>
@@ -2795,14 +2871,14 @@
       <c r="AA25" s="35"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="29">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="B26" s="30" t="s">
+      <c r="A26" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="13" t="s">
@@ -2810,11 +2886,11 @@
       </c>
       <c r="E26" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F26" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F26" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>20</v>
@@ -2822,7 +2898,7 @@
       <c r="H26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="26" t="s">
@@ -2834,7 +2910,7 @@
       <c r="L26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N26" s="27" t="s">
@@ -2843,11 +2919,15 @@
       <c r="O26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P26" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="35"/>
+      <c r="P26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S26" s="35"/>
       <c r="T26" s="35"/>
       <c r="U26" s="35"/>
@@ -2859,14 +2939,14 @@
       <c r="AA26" s="35"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="29">
+      <c r="A27" s="30">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="32" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -2874,11 +2954,11 @@
       </c>
       <c r="E27" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F27" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F27" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G27" s="26" t="s">
         <v>20</v>
@@ -2898,7 +2978,7 @@
       <c r="L27" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="34" t="s">
+      <c r="M27" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N27" s="27" t="s">
@@ -2907,11 +2987,15 @@
       <c r="O27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="35"/>
+      <c r="P27" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S27" s="35"/>
       <c r="T27" s="35"/>
       <c r="U27" s="35"/>
@@ -2923,14 +3007,14 @@
       <c r="AA27" s="35"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="29">
+      <c r="A28" s="30">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="13" t="s">
@@ -2940,9 +3024,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F28" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G28" s="26" t="s">
         <v>20</v>
@@ -2974,8 +3058,12 @@
       <c r="P28" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
+      <c r="Q28" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R28" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S28" s="35"/>
       <c r="T28" s="35"/>
       <c r="U28" s="35"/>
@@ -2987,14 +3075,14 @@
       <c r="AA28" s="35"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="29">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="30">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B29" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="32" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="13" t="s">
@@ -3002,11 +3090,11 @@
       </c>
       <c r="E29" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F29" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F29" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G29" s="26" t="s">
         <v>20</v>
@@ -3017,13 +3105,13 @@
       <c r="I29" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="34" t="s">
+      <c r="J29" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K29" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="34" t="s">
+      <c r="L29" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M29" s="26" t="s">
@@ -3035,11 +3123,15 @@
       <c r="O29" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P29" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="35"/>
+      <c r="P29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
@@ -3051,14 +3143,14 @@
       <c r="AA29" s="35"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="29">
+      <c r="A30" s="30">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="32" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="13" t="s">
@@ -3068,9 +3160,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F30" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F30" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G30" s="26" t="s">
         <v>20</v>
@@ -3090,10 +3182,10 @@
       <c r="L30" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M30" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N30" s="34" t="s">
+      <c r="M30" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N30" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O30" s="27" t="s">
@@ -3102,8 +3194,12 @@
       <c r="P30" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
+      <c r="Q30" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R30" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S30" s="35"/>
       <c r="T30" s="35"/>
       <c r="U30" s="35"/>
@@ -3115,14 +3211,14 @@
       <c r="AA30" s="35"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="29">
+      <c r="A31" s="30">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="13" t="s">
@@ -3132,9 +3228,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F31" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F31" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G31" s="26" t="s">
         <v>20</v>
@@ -3151,7 +3247,7 @@
       <c r="K31" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="34" t="s">
+      <c r="L31" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M31" s="26" t="s">
@@ -3166,8 +3262,12 @@
       <c r="P31" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="35"/>
+      <c r="Q31" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R31" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S31" s="35"/>
       <c r="T31" s="35"/>
       <c r="U31" s="35"/>
@@ -3179,14 +3279,14 @@
       <c r="AA31" s="35"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="29">
+      <c r="A32" s="30">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="32" t="s">
         <v>71</v>
       </c>
       <c r="D32" s="13" t="s">
@@ -3196,17 +3296,17 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F32" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="G32" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="34" t="s">
+      <c r="F32" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J32" s="26" t="s">
@@ -3230,8 +3330,12 @@
       <c r="P32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
+      <c r="Q32" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R32" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S32" s="35"/>
       <c r="T32" s="35"/>
       <c r="U32" s="35"/>
@@ -3243,14 +3347,14 @@
       <c r="AA32" s="35"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="29">
+      <c r="A33" s="30">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="13" t="s">
@@ -3258,11 +3362,11 @@
       </c>
       <c r="E33" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="F33" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G33" s="26" t="s">
         <v>20</v>
@@ -3294,8 +3398,12 @@
       <c r="P33" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
+      <c r="Q33" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S33" s="35"/>
       <c r="T33" s="35"/>
       <c r="U33" s="35"/>
@@ -3307,14 +3415,14 @@
       <c r="AA33" s="35"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="29">
+      <c r="A34" s="30">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="32" t="s">
         <v>75</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -3322,11 +3430,11 @@
       </c>
       <c r="E34" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F34" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F34" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>20</v>
@@ -3349,7 +3457,7 @@
       <c r="M34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N34" s="34" t="s">
+      <c r="N34" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O34" s="27" t="s">
@@ -3358,8 +3466,12 @@
       <c r="P34" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
+      <c r="Q34" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R34" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S34" s="35"/>
       <c r="T34" s="35"/>
       <c r="U34" s="35"/>
@@ -3371,14 +3483,14 @@
       <c r="AA34" s="35"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="29">
+      <c r="A35" s="30">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="13" t="s">
@@ -3386,11 +3498,11 @@
       </c>
       <c r="E35" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F35" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F35" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G35" s="26" t="s">
         <v>20</v>
@@ -3407,7 +3519,7 @@
       <c r="K35" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L35" s="34" t="s">
+      <c r="L35" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M35" s="26" t="s">
@@ -3422,8 +3534,12 @@
       <c r="P35" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
+      <c r="Q35" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S35" s="35"/>
       <c r="T35" s="35"/>
       <c r="U35" s="35"/>
@@ -3435,14 +3551,14 @@
       <c r="AA35" s="35"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="29">
+      <c r="A36" s="30">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="32" t="s">
         <v>79</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -3450,11 +3566,11 @@
       </c>
       <c r="E36" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="F36" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G36" s="26" t="s">
         <v>20</v>
@@ -3486,8 +3602,12 @@
       <c r="P36" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
+      <c r="Q36" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R36" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S36" s="35"/>
       <c r="T36" s="35"/>
       <c r="U36" s="35"/>
@@ -3499,14 +3619,14 @@
       <c r="AA36" s="35"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="29">
+      <c r="A37" s="30">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="32" t="s">
         <v>81</v>
       </c>
       <c r="D37" s="13" t="s">
@@ -3516,9 +3636,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F37" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F37" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G37" s="26" t="s">
         <v>20</v>
@@ -3550,8 +3670,12 @@
       <c r="P37" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q37" s="35"/>
-      <c r="R37" s="35"/>
+      <c r="Q37" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R37" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S37" s="35"/>
       <c r="T37" s="35"/>
       <c r="U37" s="35"/>
@@ -3563,14 +3687,14 @@
       <c r="AA37" s="35"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="29">
+      <c r="A38" s="30">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D38" s="13" t="s">
@@ -3578,19 +3702,19 @@
       </c>
       <c r="E38" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F38" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F38" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G38" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H38" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I38" s="34" t="s">
+      <c r="H38" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J38" s="26" t="s">
@@ -3614,8 +3738,12 @@
       <c r="P38" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35"/>
+      <c r="Q38" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R38" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S38" s="35"/>
       <c r="T38" s="35"/>
       <c r="U38" s="35"/>
@@ -3627,14 +3755,14 @@
       <c r="AA38" s="35"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="29">
+      <c r="A39" s="30">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="32" t="s">
         <v>85</v>
       </c>
       <c r="D39" s="13" t="s">
@@ -3644,9 +3772,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F39" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F39" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G39" s="26" t="s">
         <v>20</v>
@@ -3654,7 +3782,7 @@
       <c r="H39" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J39" s="26" t="s">
@@ -3678,8 +3806,12 @@
       <c r="P39" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
+      <c r="Q39" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R39" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S39" s="35"/>
       <c r="T39" s="35"/>
       <c r="U39" s="35"/>
@@ -3691,14 +3823,14 @@
       <c r="AA39" s="35"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="29">
+      <c r="A40" s="30">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="32" t="s">
         <v>87</v>
       </c>
       <c r="D40" s="13" t="s">
@@ -3706,11 +3838,11 @@
       </c>
       <c r="E40" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F40" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F40" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G40" s="26" t="s">
         <v>20</v>
@@ -3721,7 +3853,7 @@
       <c r="I40" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="34" t="s">
+      <c r="J40" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K40" s="26" t="s">
@@ -3733,7 +3865,7 @@
       <c r="M40" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N40" s="34" t="s">
+      <c r="N40" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O40" s="27" t="s">
@@ -3742,8 +3874,12 @@
       <c r="P40" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
+      <c r="Q40" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R40" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S40" s="35"/>
       <c r="T40" s="35"/>
       <c r="U40" s="35"/>
@@ -3755,14 +3891,14 @@
       <c r="AA40" s="35"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="29">
+      <c r="A41" s="30">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D41" s="13" t="s">
@@ -3772,9 +3908,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F41" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="F41" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G41" s="26" t="s">
         <v>20</v>
@@ -3785,19 +3921,19 @@
       <c r="I41" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="34" t="s">
+      <c r="J41" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K41" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L41" s="34" t="s">
+      <c r="L41" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M41" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N41" s="34" t="s">
+      <c r="N41" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O41" s="27" t="s">
@@ -3806,8 +3942,12 @@
       <c r="P41" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
+      <c r="Q41" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R41" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S41" s="35"/>
       <c r="T41" s="35"/>
       <c r="U41" s="35"/>
@@ -3819,14 +3959,14 @@
       <c r="AA41" s="35"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="29">
+      <c r="A42" s="30">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D42" s="13" t="s">
@@ -3836,11 +3976,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F42" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="G42" s="33" t="s">
+      <c r="F42" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G42" s="34" t="s">
         <v>23</v>
       </c>
       <c r="H42" s="26" t="s">
@@ -3849,7 +3989,7 @@
       <c r="I42" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="34" t="s">
+      <c r="J42" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K42" s="26" t="s">
@@ -3861,7 +4001,7 @@
       <c r="M42" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N42" s="34" t="s">
+      <c r="N42" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O42" s="27" t="s">
@@ -3870,8 +4010,12 @@
       <c r="P42" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="35"/>
+      <c r="Q42" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R42" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S42" s="35"/>
       <c r="T42" s="35"/>
       <c r="U42" s="35"/>
@@ -3883,14 +4027,14 @@
       <c r="AA42" s="35"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="29">
+      <c r="A43" s="30">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="32" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="13" t="s">
@@ -3898,11 +4042,11 @@
       </c>
       <c r="E43" s="24">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F43" s="32">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F43" s="33">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="G43" s="26" t="s">
         <v>20</v>
@@ -3910,16 +4054,16 @@
       <c r="H43" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I43" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" s="34" t="s">
+      <c r="I43" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K43" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L43" s="34" t="s">
+      <c r="L43" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M43" s="26" t="s">
@@ -3931,11 +4075,15 @@
       <c r="O43" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P43" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="35"/>
+      <c r="P43" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q43" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R43" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S43" s="35"/>
       <c r="T43" s="35"/>
       <c r="U43" s="35"/>
@@ -3947,14 +4095,14 @@
       <c r="AA43" s="35"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="29">
+      <c r="A44" s="30">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="32" t="s">
         <v>95</v>
       </c>
       <c r="D44" s="13" t="s">
@@ -3962,11 +4110,11 @@
       </c>
       <c r="E44" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F44" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F44" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G44" s="26" t="s">
         <v>20</v>
@@ -3977,7 +4125,7 @@
       <c r="I44" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="34" t="s">
+      <c r="J44" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K44" s="26" t="s">
@@ -3998,8 +4146,12 @@
       <c r="P44" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q44" s="35"/>
-      <c r="R44" s="35"/>
+      <c r="Q44" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R44" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S44" s="35"/>
       <c r="T44" s="35"/>
       <c r="U44" s="35"/>
@@ -4011,14 +4163,14 @@
       <c r="AA44" s="35"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="29">
+      <c r="A45" s="30">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="32" t="s">
         <v>97</v>
       </c>
       <c r="D45" s="13" t="s">
@@ -4028,14 +4180,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F45" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F45" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G45" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I45" s="26" t="s">
@@ -4059,11 +4211,15 @@
       <c r="O45" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P45" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q45" s="35"/>
-      <c r="R45" s="35"/>
+      <c r="P45" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q45" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R45" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S45" s="35"/>
       <c r="T45" s="35"/>
       <c r="U45" s="35"/>
@@ -4075,14 +4231,14 @@
       <c r="AA45" s="35"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="29">
+      <c r="A46" s="30">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="32" t="s">
         <v>99</v>
       </c>
       <c r="D46" s="13" t="s">
@@ -4090,11 +4246,11 @@
       </c>
       <c r="E46" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F46" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F46" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G46" s="26" t="s">
         <v>20</v>
@@ -4102,16 +4258,16 @@
       <c r="H46" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I46" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J46" s="34" t="s">
+      <c r="I46" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K46" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L46" s="34" t="s">
+      <c r="L46" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M46" s="26" t="s">
@@ -4126,8 +4282,12 @@
       <c r="P46" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="35"/>
+      <c r="Q46" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R46" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S46" s="35"/>
       <c r="T46" s="35"/>
       <c r="U46" s="35"/>
@@ -4139,14 +4299,14 @@
       <c r="AA46" s="35"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="29">
+      <c r="A47" s="30">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="32" t="s">
         <v>101</v>
       </c>
       <c r="D47" s="13" t="s">
@@ -4154,11 +4314,11 @@
       </c>
       <c r="E47" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F47" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F47" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>20</v>
@@ -4166,7 +4326,7 @@
       <c r="H47" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I47" s="34" t="s">
+      <c r="I47" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J47" s="26" t="s">
@@ -4175,7 +4335,7 @@
       <c r="K47" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L47" s="34" t="s">
+      <c r="L47" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M47" s="26" t="s">
@@ -4190,8 +4350,12 @@
       <c r="P47" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q47" s="35"/>
-      <c r="R47" s="35"/>
+      <c r="Q47" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R47" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S47" s="35"/>
       <c r="T47" s="35"/>
       <c r="U47" s="35"/>
@@ -4203,14 +4367,14 @@
       <c r="AA47" s="35"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="29">
+      <c r="A48" s="30">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="32" t="s">
         <v>103</v>
       </c>
       <c r="D48" s="13" t="s">
@@ -4220,9 +4384,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F48" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F48" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>20</v>
@@ -4254,8 +4418,12 @@
       <c r="P48" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q48" s="35"/>
-      <c r="R48" s="35"/>
+      <c r="Q48" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R48" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S48" s="35"/>
       <c r="T48" s="35"/>
       <c r="U48" s="35"/>
@@ -4267,14 +4435,14 @@
       <c r="AA48" s="35"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="29">
+      <c r="A49" s="30">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="32" t="s">
         <v>105</v>
       </c>
       <c r="D49" s="13" t="s">
@@ -4284,9 +4452,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F49" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F49" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G49" s="26" t="s">
         <v>20</v>
@@ -4294,7 +4462,7 @@
       <c r="H49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I49" s="34" t="s">
+      <c r="I49" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J49" s="26" t="s">
@@ -4306,7 +4474,7 @@
       <c r="L49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M49" s="34" t="s">
+      <c r="M49" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N49" s="27" t="s">
@@ -4318,8 +4486,12 @@
       <c r="P49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q49" s="35"/>
-      <c r="R49" s="35"/>
+      <c r="Q49" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R49" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S49" s="35"/>
       <c r="T49" s="35"/>
       <c r="U49" s="35"/>
@@ -4331,14 +4503,14 @@
       <c r="AA49" s="35"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="29">
+      <c r="A50" s="30">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="32" t="s">
         <v>107</v>
       </c>
       <c r="D50" s="13" t="s">
@@ -4346,11 +4518,11 @@
       </c>
       <c r="E50" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F50" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F50" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G50" s="26" t="s">
         <v>20</v>
@@ -4367,7 +4539,7 @@
       <c r="K50" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L50" s="34" t="s">
+      <c r="L50" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M50" s="26" t="s">
@@ -4382,8 +4554,12 @@
       <c r="P50" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q50" s="35"/>
-      <c r="R50" s="35"/>
+      <c r="Q50" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R50" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S50" s="35"/>
       <c r="T50" s="35"/>
       <c r="U50" s="35"/>
@@ -4395,14 +4571,14 @@
       <c r="AA50" s="35"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="29">
+      <c r="A51" s="30">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="32" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="13" t="s">
@@ -4410,11 +4586,11 @@
       </c>
       <c r="E51" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F51" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F51" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G51" s="26" t="s">
         <v>20</v>
@@ -4428,16 +4604,16 @@
       <c r="J51" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="K51" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="L51" s="34" t="s">
+      <c r="K51" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L51" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M51" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N51" s="34" t="s">
+      <c r="N51" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O51" s="27" t="s">
@@ -4446,8 +4622,12 @@
       <c r="P51" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
+      <c r="Q51" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R51" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S51" s="35"/>
       <c r="T51" s="35"/>
       <c r="U51" s="35"/>
@@ -4459,14 +4639,14 @@
       <c r="AA51" s="35"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="29">
+      <c r="A52" s="30">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="32" t="s">
         <v>111</v>
       </c>
       <c r="D52" s="13" t="s">
@@ -4474,9 +4654,9 @@
       </c>
       <c r="E52" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="32">
+        <v>2</v>
+      </c>
+      <c r="F52" s="33">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -4510,8 +4690,12 @@
       <c r="P52" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q52" s="35"/>
-      <c r="R52" s="35"/>
+      <c r="Q52" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R52" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S52" s="35"/>
       <c r="T52" s="35"/>
       <c r="U52" s="35"/>
@@ -4523,14 +4707,14 @@
       <c r="AA52" s="35"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="29">
+      <c r="A53" s="30">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="32" t="s">
         <v>113</v>
       </c>
       <c r="D53" s="13" t="s">
@@ -4540,9 +4724,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F53" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="F53" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G53" s="26" t="s">
         <v>20</v>
@@ -4553,13 +4737,13 @@
       <c r="I53" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J53" s="34" t="s">
+      <c r="J53" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K53" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L53" s="34" t="s">
+      <c r="L53" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M53" s="26" t="s">
@@ -4571,11 +4755,15 @@
       <c r="O53" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P53" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q53" s="35"/>
-      <c r="R53" s="35"/>
+      <c r="P53" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q53" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R53" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S53" s="35"/>
       <c r="T53" s="35"/>
       <c r="U53" s="35"/>
@@ -4587,14 +4775,14 @@
       <c r="AA53" s="35"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="29">
+      <c r="A54" s="30">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="32" t="s">
         <v>115</v>
       </c>
       <c r="D54" s="13" t="s">
@@ -4602,44 +4790,48 @@
       </c>
       <c r="E54" s="24">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="F54" s="32">
+        <v>11</v>
+      </c>
+      <c r="F54" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G54" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J54" s="34" t="s">
+      <c r="G54" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J54" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K54" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="M54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q54" s="35"/>
-      <c r="R54" s="35"/>
+      <c r="L54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q54" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R54" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S54" s="35"/>
       <c r="T54" s="35"/>
       <c r="U54" s="35"/>
@@ -4651,14 +4843,14 @@
       <c r="AA54" s="35"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="29">
+      <c r="A55" s="30">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="32" t="s">
         <v>117</v>
       </c>
       <c r="D55" s="13" t="s">
@@ -4668,9 +4860,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F55" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F55" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G55" s="26" t="s">
         <v>20</v>
@@ -4690,10 +4882,10 @@
       <c r="L55" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M55" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N55" s="34" t="s">
+      <c r="M55" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N55" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O55" s="27" t="s">
@@ -4702,8 +4894,12 @@
       <c r="P55" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q55" s="35"/>
-      <c r="R55" s="35"/>
+      <c r="Q55" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R55" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S55" s="35"/>
       <c r="T55" s="35"/>
       <c r="U55" s="35"/>
@@ -4715,14 +4911,14 @@
       <c r="AA55" s="35"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="29">
+      <c r="A56" s="30">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="32" t="s">
         <v>119</v>
       </c>
       <c r="D56" s="13" t="s">
@@ -4732,9 +4928,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F56" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F56" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G56" s="26" t="s">
         <v>20</v>
@@ -4766,8 +4962,12 @@
       <c r="P56" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q56" s="35"/>
-      <c r="R56" s="35"/>
+      <c r="Q56" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R56" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S56" s="35"/>
       <c r="T56" s="35"/>
       <c r="U56" s="35"/>
@@ -4779,14 +4979,14 @@
       <c r="AA56" s="35"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="29">
+      <c r="A57" s="30">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="32" t="s">
         <v>121</v>
       </c>
       <c r="D57" s="13" t="s">
@@ -4796,9 +4996,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F57" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F57" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G57" s="26" t="s">
         <v>20</v>
@@ -4806,7 +5006,7 @@
       <c r="H57" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I57" s="34" t="s">
+      <c r="I57" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J57" s="26" t="s">
@@ -4830,8 +5030,12 @@
       <c r="P57" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="35"/>
+      <c r="Q57" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R57" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S57" s="35"/>
       <c r="T57" s="35"/>
       <c r="U57" s="35"/>
@@ -4843,14 +5047,14 @@
       <c r="AA57" s="35"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="29">
+      <c r="A58" s="30">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="32" t="s">
         <v>123</v>
       </c>
       <c r="D58" s="13" t="s">
@@ -4860,11 +5064,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F58" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="G58" s="33" t="s">
+      <c r="F58" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G58" s="34" t="s">
         <v>23</v>
       </c>
       <c r="H58" s="26" t="s">
@@ -4891,11 +5095,15 @@
       <c r="O58" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P58" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q58" s="35"/>
-      <c r="R58" s="35"/>
+      <c r="P58" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q58" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R58" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S58" s="35"/>
       <c r="T58" s="35"/>
       <c r="U58" s="35"/>
@@ -4907,14 +5115,14 @@
       <c r="AA58" s="35"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="29">
+      <c r="A59" s="30">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="31" t="s">
+      <c r="C59" s="32" t="s">
         <v>125</v>
       </c>
       <c r="D59" s="13" t="s">
@@ -4924,9 +5132,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F59" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F59" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G59" s="26" t="s">
         <v>20</v>
@@ -4949,7 +5157,7 @@
       <c r="M59" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N59" s="34" t="s">
+      <c r="N59" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O59" s="27" t="s">
@@ -4958,8 +5166,12 @@
       <c r="P59" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q59" s="35"/>
-      <c r="R59" s="35"/>
+      <c r="Q59" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R59" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S59" s="35"/>
       <c r="T59" s="35"/>
       <c r="U59" s="35"/>
@@ -4971,14 +5183,14 @@
       <c r="AA59" s="35"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="29">
+      <c r="A60" s="30">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="32" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="13" t="s">
@@ -4986,22 +5198,22 @@
       </c>
       <c r="E60" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F60" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F60" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G60" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H60" s="34" t="s">
+      <c r="H60" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I60" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J60" s="34" t="s">
+      <c r="J60" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K60" s="26" t="s">
@@ -5016,14 +5228,18 @@
       <c r="N60" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O60" s="34" t="s">
+      <c r="O60" s="28" t="s">
         <v>23</v>
       </c>
       <c r="P60" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q60" s="35"/>
-      <c r="R60" s="35"/>
+      <c r="Q60" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R60" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S60" s="35"/>
       <c r="T60" s="35"/>
       <c r="U60" s="35"/>
@@ -5035,14 +5251,14 @@
       <c r="AA60" s="35"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="29">
+      <c r="A61" s="30">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="31" t="s">
+      <c r="C61" s="32" t="s">
         <v>129</v>
       </c>
       <c r="D61" s="13" t="s">
@@ -5052,9 +5268,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F61" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F61" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G61" s="26" t="s">
         <v>20</v>
@@ -5086,8 +5302,12 @@
       <c r="P61" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q61" s="35"/>
-      <c r="R61" s="35"/>
+      <c r="Q61" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R61" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S61" s="35"/>
       <c r="T61" s="35"/>
       <c r="U61" s="35"/>
@@ -5099,14 +5319,14 @@
       <c r="AA61" s="35"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="29">
+      <c r="A62" s="30">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C62" s="32" t="s">
         <v>131</v>
       </c>
       <c r="D62" s="13" t="s">
@@ -5116,29 +5336,29 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F62" s="32">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="G62" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H62" s="34" t="s">
+      <c r="F62" s="33">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H62" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I62" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J62" s="34" t="s">
+      <c r="J62" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K62" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L62" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="M62" s="34" t="s">
+      <c r="L62" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M62" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N62" s="27" t="s">
@@ -5150,8 +5370,12 @@
       <c r="P62" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="35"/>
+      <c r="Q62" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R62" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S62" s="35"/>
       <c r="T62" s="35"/>
       <c r="U62" s="35"/>
@@ -5163,14 +5387,14 @@
       <c r="AA62" s="35"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="29">
+      <c r="A63" s="30">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" s="32" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="13" t="s">
@@ -5178,13 +5402,13 @@
       </c>
       <c r="E63" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F63" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="G63" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G63" s="34" t="s">
         <v>23</v>
       </c>
       <c r="H63" s="26" t="s">
@@ -5214,8 +5438,12 @@
       <c r="P63" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q63" s="35"/>
-      <c r="R63" s="35"/>
+      <c r="Q63" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R63" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S63" s="35"/>
       <c r="T63" s="35"/>
       <c r="U63" s="35"/>
@@ -5227,14 +5455,14 @@
       <c r="AA63" s="35"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="29">
+      <c r="A64" s="30">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="32" t="s">
         <v>135</v>
       </c>
       <c r="D64" s="13" t="s">
@@ -5244,9 +5472,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F64" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F64" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G64" s="26" t="s">
         <v>20</v>
@@ -5272,14 +5500,18 @@
       <c r="N64" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O64" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P64" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="35"/>
+      <c r="O64" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P64" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q64" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R64" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S64" s="35"/>
       <c r="T64" s="35"/>
       <c r="U64" s="35"/>
@@ -5291,14 +5523,14 @@
       <c r="AA64" s="35"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="29">
+      <c r="A65" s="30">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="C65" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D65" s="13" t="s">
@@ -5308,14 +5540,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F65" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="G65" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H65" s="34" t="s">
+      <c r="F65" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G65" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H65" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I65" s="26" t="s">
@@ -5342,8 +5574,12 @@
       <c r="P65" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q65" s="35"/>
-      <c r="R65" s="35"/>
+      <c r="Q65" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R65" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S65" s="35"/>
       <c r="T65" s="35"/>
       <c r="U65" s="35"/>
@@ -5355,14 +5591,14 @@
       <c r="AA65" s="35"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="29">
+      <c r="A66" s="30">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="31" t="s">
+      <c r="C66" s="32" t="s">
         <v>139</v>
       </c>
       <c r="D66" s="13" t="s">
@@ -5372,9 +5608,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F66" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F66" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G66" s="26" t="s">
         <v>20</v>
@@ -5382,7 +5618,7 @@
       <c r="H66" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I66" s="34" t="s">
+      <c r="I66" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J66" s="26" t="s">
@@ -5403,11 +5639,15 @@
       <c r="O66" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P66" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q66" s="35"/>
-      <c r="R66" s="35"/>
+      <c r="P66" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q66" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R66" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S66" s="35"/>
       <c r="T66" s="35"/>
       <c r="U66" s="35"/>
@@ -5419,14 +5659,14 @@
       <c r="AA66" s="35"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="29">
+      <c r="A67" s="30">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C67" s="32" t="s">
         <v>141</v>
       </c>
       <c r="D67" s="13" t="s">
@@ -5434,11 +5674,11 @@
       </c>
       <c r="E67" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F67" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="F67" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G67" s="26" t="s">
         <v>20</v>
@@ -5467,11 +5707,15 @@
       <c r="O67" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P67" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q67" s="35"/>
-      <c r="R67" s="35"/>
+      <c r="P67" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q67" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R67" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S67" s="35"/>
       <c r="T67" s="35"/>
       <c r="U67" s="35"/>
@@ -5483,14 +5727,14 @@
       <c r="AA67" s="35"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="29">
+      <c r="A68" s="30">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="32" t="s">
         <v>143</v>
       </c>
       <c r="D68" s="13" t="s">
@@ -5500,9 +5744,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F68" s="32">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="F68" s="33">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G68" s="26" t="s">
         <v>20</v>
@@ -5534,8 +5778,12 @@
       <c r="P68" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q68" s="35"/>
-      <c r="R68" s="35"/>
+      <c r="Q68" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R68" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S68" s="35"/>
       <c r="T68" s="35"/>
       <c r="U68" s="35"/>
@@ -5547,14 +5795,14 @@
       <c r="AA68" s="35"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="29">
+      <c r="A69" s="30">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="31" t="s">
+      <c r="C69" s="32" t="s">
         <v>145</v>
       </c>
       <c r="D69" s="13" t="s">
@@ -5562,11 +5810,11 @@
       </c>
       <c r="E69" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F69" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F69" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G69" s="26" t="s">
         <v>20</v>
@@ -5583,7 +5831,7 @@
       <c r="K69" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="34" t="s">
+      <c r="L69" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M69" s="26" t="s">
@@ -5595,11 +5843,15 @@
       <c r="O69" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P69" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q69" s="35"/>
-      <c r="R69" s="35"/>
+      <c r="P69" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q69" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R69" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S69" s="35"/>
       <c r="T69" s="35"/>
       <c r="U69" s="35"/>
@@ -5611,14 +5863,14 @@
       <c r="AA69" s="35"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="29">
+      <c r="A70" s="30">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="31" t="s">
+      <c r="C70" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D70" s="13" t="s">
@@ -5626,11 +5878,11 @@
       </c>
       <c r="E70" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F70" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F70" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G70" s="26" t="s">
         <v>20</v>
@@ -5638,7 +5890,7 @@
       <c r="H70" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I70" s="34" t="s">
+      <c r="I70" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J70" s="26" t="s">
@@ -5650,7 +5902,7 @@
       <c r="L70" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M70" s="34" t="s">
+      <c r="M70" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N70" s="27" t="s">
@@ -5659,11 +5911,15 @@
       <c r="O70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P70" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q70" s="35"/>
-      <c r="R70" s="35"/>
+      <c r="P70" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q70" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R70" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S70" s="35"/>
       <c r="T70" s="35"/>
       <c r="U70" s="35"/>
@@ -5675,14 +5931,14 @@
       <c r="AA70" s="35"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="29">
+      <c r="A71" s="30">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="31" t="s">
+      <c r="C71" s="32" t="s">
         <v>149</v>
       </c>
       <c r="D71" s="13" t="s">
@@ -5690,11 +5946,11 @@
       </c>
       <c r="E71" s="24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F71" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="F71" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G71" s="26" t="s">
         <v>20</v>
@@ -5714,10 +5970,10 @@
       <c r="L71" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M71" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="N71" s="34" t="s">
+      <c r="M71" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N71" s="28" t="s">
         <v>23</v>
       </c>
       <c r="O71" s="27" t="s">
@@ -5726,8 +5982,12 @@
       <c r="P71" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q71" s="35"/>
-      <c r="R71" s="35"/>
+      <c r="Q71" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R71" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S71" s="35"/>
       <c r="T71" s="35"/>
       <c r="U71" s="35"/>
@@ -5739,14 +5999,14 @@
       <c r="AA71" s="35"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="29">
+      <c r="A72" s="30">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="C72" s="31" t="s">
+      <c r="C72" s="32" t="s">
         <v>151</v>
       </c>
       <c r="D72" s="13" t="s">
@@ -5756,26 +6016,26 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F72" s="32">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="G72" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H72" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I72" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J72" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="K72" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="L72" s="34" t="s">
+      <c r="F72" s="33">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G72" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H72" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I72" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J72" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K72" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L72" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M72" s="26" t="s">
@@ -5790,8 +6050,12 @@
       <c r="P72" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q72" s="35"/>
-      <c r="R72" s="35"/>
+      <c r="Q72" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R72" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S72" s="35"/>
       <c r="T72" s="35"/>
       <c r="U72" s="35"/>
@@ -5803,14 +6067,14 @@
       <c r="AA72" s="35"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="29">
+      <c r="A73" s="30">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C73" s="31" t="s">
+      <c r="C73" s="32" t="s">
         <v>153</v>
       </c>
       <c r="D73" s="13" t="s">
@@ -5820,14 +6084,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F73" s="32">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="G73" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H73" s="34" t="s">
+      <c r="F73" s="33">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G73" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H73" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I73" s="26" t="s">
@@ -5845,17 +6109,21 @@
       <c r="M73" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N73" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O73" s="34" t="s">
+      <c r="N73" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O73" s="28" t="s">
         <v>23</v>
       </c>
       <c r="P73" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q73" s="35"/>
-      <c r="R73" s="35"/>
+      <c r="Q73" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R73" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S73" s="35"/>
       <c r="T73" s="35"/>
       <c r="U73" s="35"/>
@@ -5867,14 +6135,14 @@
       <c r="AA73" s="35"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="29">
+      <c r="A74" s="30">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C74" s="31" t="s">
+      <c r="C74" s="32" t="s">
         <v>155</v>
       </c>
       <c r="D74" s="13" t="s">
@@ -5884,14 +6152,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F74" s="32">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="F74" s="33">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H74" s="34" t="s">
+      <c r="H74" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I74" s="26" t="s">
@@ -5918,8 +6186,12 @@
       <c r="P74" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q74" s="35"/>
-      <c r="R74" s="35"/>
+      <c r="Q74" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R74" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S74" s="35"/>
       <c r="T74" s="35"/>
       <c r="U74" s="35"/>
@@ -5931,14 +6203,14 @@
       <c r="AA74" s="35"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="29">
+      <c r="A75" s="30">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="C75" s="31" t="s">
+      <c r="C75" s="32" t="s">
         <v>157</v>
       </c>
       <c r="D75" s="13" t="s">
@@ -5948,9 +6220,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F75" s="32">
-        <f t="shared" si="2"/>
-        <v>8</v>
+      <c r="F75" s="33">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G75" s="26" t="s">
         <v>20</v>
@@ -5964,7 +6236,7 @@
       <c r="J75" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="K75" s="34" t="s">
+      <c r="K75" s="28" t="s">
         <v>23</v>
       </c>
       <c r="L75" s="26" t="s">
@@ -5976,14 +6248,18 @@
       <c r="N75" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O75" s="34" t="s">
+      <c r="O75" s="28" t="s">
         <v>23</v>
       </c>
       <c r="P75" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q75" s="35"/>
-      <c r="R75" s="35"/>
+      <c r="Q75" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R75" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S75" s="35"/>
       <c r="T75" s="35"/>
       <c r="U75" s="35"/>
@@ -5995,14 +6271,14 @@
       <c r="AA75" s="35"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="29">
+      <c r="A76" s="30">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C76" s="31" t="s">
+      <c r="C76" s="32" t="s">
         <v>159</v>
       </c>
       <c r="D76" s="13" t="s">
@@ -6012,17 +6288,17 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F76" s="32">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="G76" s="33" t="s">
+      <c r="F76" s="33">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G76" s="34" t="s">
         <v>23</v>
       </c>
       <c r="H76" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I76" s="34" t="s">
+      <c r="I76" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J76" s="26" t="s">
@@ -6031,7 +6307,7 @@
       <c r="K76" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="34" t="s">
+      <c r="L76" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M76" s="26" t="s">
@@ -6046,8 +6322,12 @@
       <c r="P76" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q76" s="35"/>
-      <c r="R76" s="35"/>
+      <c r="Q76" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R76" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="S76" s="35"/>
       <c r="T76" s="35"/>
       <c r="U76" s="35"/>
@@ -6059,14 +6339,14 @@
       <c r="AA76" s="35"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="29">
+      <c r="A77" s="30">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="31" t="s">
+      <c r="C77" s="32" t="s">
         <v>161</v>
       </c>
       <c r="D77" s="13" t="s">
@@ -6074,9 +6354,9 @@
       </c>
       <c r="E77" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F77" s="32">
+        <v>5</v>
+      </c>
+      <c r="F77" s="33">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -6086,10 +6366,10 @@
       <c r="H77" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I77" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J77" s="34" t="s">
+      <c r="I77" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J77" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K77" s="26" t="s">
@@ -6098,7 +6378,7 @@
       <c r="L77" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M77" s="34" t="s">
+      <c r="M77" s="28" t="s">
         <v>23</v>
       </c>
       <c r="N77" s="27" t="s">
@@ -6110,8 +6390,12 @@
       <c r="P77" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q77" s="35"/>
-      <c r="R77" s="35"/>
+      <c r="Q77" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R77" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="S77" s="35"/>
       <c r="T77" s="35"/>
       <c r="U77" s="35"/>
@@ -6123,18 +6407,18 @@
       <c r="AA77" s="35"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
+      <c r="A78" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B78" s="31"/>
+      <c r="C78" s="32"/>
       <c r="D78" s="36"/>
       <c r="E78" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F78" s="32" t="str">
+      <c r="F78" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6161,18 +6445,18 @@
       <c r="AA78" s="35"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B79" s="30"/>
-      <c r="C79" s="31"/>
+      <c r="A79" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B79" s="31"/>
+      <c r="C79" s="32"/>
       <c r="D79" s="36"/>
       <c r="E79" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F79" s="32" t="str">
+      <c r="F79" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6199,18 +6483,18 @@
       <c r="AA79" s="35"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B80" s="30"/>
-      <c r="C80" s="31"/>
+      <c r="A80" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B80" s="31"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="24"/>
       <c r="E80" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F80" s="32" t="str">
+      <c r="F80" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6237,18 +6521,18 @@
       <c r="AA80" s="35"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B81" s="30"/>
-      <c r="C81" s="31"/>
+      <c r="A81" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B81" s="31"/>
+      <c r="C81" s="32"/>
       <c r="D81" s="24"/>
       <c r="E81" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F81" s="32" t="str">
+      <c r="F81" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6275,18 +6559,18 @@
       <c r="AA81" s="35"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B82" s="30"/>
-      <c r="C82" s="31"/>
+      <c r="A82" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B82" s="31"/>
+      <c r="C82" s="32"/>
       <c r="D82" s="24"/>
       <c r="E82" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F82" s="32" t="str">
+      <c r="F82" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6313,18 +6597,18 @@
       <c r="AA82" s="35"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B83" s="30"/>
-      <c r="C83" s="31"/>
+      <c r="A83" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B83" s="31"/>
+      <c r="C83" s="32"/>
       <c r="D83" s="24"/>
       <c r="E83" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F83" s="32" t="str">
+      <c r="F83" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6351,18 +6635,18 @@
       <c r="AA83" s="35"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B84" s="30"/>
-      <c r="C84" s="31"/>
+      <c r="A84" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B84" s="31"/>
+      <c r="C84" s="32"/>
       <c r="D84" s="24"/>
       <c r="E84" s="24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F84" s="32" t="str">
+      <c r="F84" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6389,7 +6673,7 @@
       <c r="AA84" s="35"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="29" t="str">
+      <c r="A85" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6400,7 +6684,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F85" s="32" t="str">
+      <c r="F85" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6427,7 +6711,7 @@
       <c r="AA85" s="35"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="29" t="str">
+      <c r="A86" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6438,7 +6722,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F86" s="32" t="str">
+      <c r="F86" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6465,7 +6749,7 @@
       <c r="AA86" s="35"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="29" t="str">
+      <c r="A87" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6476,7 +6760,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F87" s="32" t="str">
+      <c r="F87" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6503,7 +6787,7 @@
       <c r="AA87" s="35"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="29" t="str">
+      <c r="A88" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6514,7 +6798,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F88" s="32" t="str">
+      <c r="F88" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6541,7 +6825,7 @@
       <c r="AA88" s="35"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="29" t="str">
+      <c r="A89" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6552,7 +6836,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F89" s="32" t="str">
+      <c r="F89" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6579,7 +6863,7 @@
       <c r="AA89" s="35"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="29" t="str">
+      <c r="A90" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6590,7 +6874,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F90" s="32" t="str">
+      <c r="F90" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6617,7 +6901,7 @@
       <c r="AA90" s="35"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="29" t="str">
+      <c r="A91" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6628,7 +6912,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F91" s="32" t="str">
+      <c r="F91" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6655,7 +6939,7 @@
       <c r="AA91" s="35"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="29" t="str">
+      <c r="A92" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6666,7 +6950,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F92" s="32" t="str">
+      <c r="F92" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6693,7 +6977,7 @@
       <c r="AA92" s="35"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="29" t="str">
+      <c r="A93" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6704,7 +6988,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F93" s="32" t="str">
+      <c r="F93" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6731,7 +7015,7 @@
       <c r="AA93" s="35"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="29" t="str">
+      <c r="A94" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6742,7 +7026,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F94" s="32" t="str">
+      <c r="F94" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6769,7 +7053,7 @@
       <c r="AA94" s="35"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="29" t="str">
+      <c r="A95" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -6780,7 +7064,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F95" s="32" t="str">
+      <c r="F95" s="33" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>